<commit_message>
Integrating the pre-treatment of statutory rates
</commit_message>
<xml_diff>
--- a/tax_deficit_simulator/data/KPMG_statutoryrates.xlsx
+++ b/tax_deficit_simulator/data/KPMG_statutoryrates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Theresa Neef\Dropbox\EUTO\studies\2_tax_deficit\3_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Theresa Neef\Dropbox\EUTO\Studies\2_tax_deficit\4_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65B92BF3-81A0-4404-A9A6-095A89C7B2A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEC0194-2022-47E6-9160-27EF2480C135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{EBC55262-2934-4873-B718-DDCE411EB7C1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EBC55262-2934-4873-B718-DDCE411EB7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="210">
   <si>
     <t>CODE</t>
   </si>
@@ -48,186 +48,87 @@
     <t>Country</t>
   </si>
   <si>
-    <t>country_code</t>
-  </si>
-  <si>
-    <t>Partner country</t>
-  </si>
-  <si>
-    <t>missing data</t>
-  </si>
-  <si>
     <t>Aruba</t>
   </si>
   <si>
-    <t>ANT</t>
-  </si>
-  <si>
-    <t>Netherlands antilles</t>
-  </si>
-  <si>
     <t>Afghanistan</t>
   </si>
   <si>
-    <t>ASM</t>
-  </si>
-  <si>
-    <t>American Samoa</t>
-  </si>
-  <si>
     <t>AFRICA</t>
   </si>
   <si>
     <t>Africa average</t>
   </si>
   <si>
-    <t>AZE</t>
-  </si>
-  <si>
     <t>Azerbaijan</t>
   </si>
   <si>
     <t>Angola</t>
   </si>
   <si>
-    <t>BVT</t>
-  </si>
-  <si>
-    <t>Bouvet Island</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
     <t>Anguilla</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>FRO</t>
-  </si>
-  <si>
-    <t>Faroe Islands</t>
-  </si>
-  <si>
     <t>Albania</t>
   </si>
   <si>
-    <t>IRN</t>
-  </si>
-  <si>
-    <t>Iran</t>
-  </si>
-  <si>
     <t>AMERICA</t>
   </si>
   <si>
     <t>Americas average</t>
   </si>
   <si>
-    <t>PRI</t>
-  </si>
-  <si>
-    <t>Puerto Rico</t>
-  </si>
-  <si>
     <t>Andorra</t>
   </si>
   <si>
     <t>CIV</t>
   </si>
   <si>
-    <t>cote d'ivoire</t>
-  </si>
-  <si>
     <t>United Arab Emirates</t>
   </si>
   <si>
-    <t>NIC</t>
-  </si>
-  <si>
     <t>Nicaragua</t>
   </si>
   <si>
     <t>Argentina</t>
   </si>
   <si>
-    <t>GRL</t>
-  </si>
-  <si>
-    <t>Greenland</t>
-  </si>
-  <si>
     <t>Armenia</t>
   </si>
   <si>
-    <t>GUM</t>
-  </si>
-  <si>
-    <t>Guam</t>
-  </si>
-  <si>
     <t>ASIA</t>
   </si>
   <si>
     <t>Asia average</t>
   </si>
   <si>
-    <t>MCO</t>
-  </si>
-  <si>
     <t>Monaco</t>
   </si>
   <si>
     <t>Antigua and Barbuda</t>
   </si>
   <si>
-    <t>SSD</t>
-  </si>
-  <si>
-    <t>South Sudan</t>
-  </si>
-  <si>
     <t>Australia</t>
   </si>
   <si>
-    <t>ETH</t>
-  </si>
-  <si>
     <t>Ethiopia</t>
   </si>
   <si>
     <t>Austria</t>
   </si>
   <si>
-    <t>LAO</t>
-  </si>
-  <si>
-    <t>Lao People's Democratic Republic</t>
-  </si>
-  <si>
-    <t>MMR</t>
-  </si>
-  <si>
     <t>Myanmar</t>
   </si>
   <si>
     <t>Burundi</t>
   </si>
   <si>
-    <t>BTN</t>
-  </si>
-  <si>
-    <t>Bhutan</t>
-  </si>
-  <si>
     <t>Belgium</t>
   </si>
   <si>
-    <t>BFA</t>
-  </si>
-  <si>
     <t>Burkina Faso</t>
   </si>
   <si>
@@ -240,219 +141,99 @@
     <t>Congo</t>
   </si>
   <si>
-    <t>GAB</t>
-  </si>
-  <si>
     <t>Gabon</t>
   </si>
   <si>
     <t>Bangladesh</t>
   </si>
   <si>
-    <t>GUY</t>
-  </si>
-  <si>
-    <t>Guyana</t>
-  </si>
-  <si>
     <t>Bulgaria</t>
   </si>
   <si>
-    <t>LBR</t>
-  </si>
-  <si>
-    <t>Liberia</t>
-  </si>
-  <si>
     <t>Bahrain</t>
   </si>
   <si>
-    <t>MDG</t>
-  </si>
-  <si>
     <t>Madagascar</t>
   </si>
   <si>
     <t>Bahamas</t>
   </si>
   <si>
-    <t>MDV</t>
-  </si>
-  <si>
-    <t>Maldives</t>
-  </si>
-  <si>
     <t>Bosnia and Herzegovina</t>
   </si>
   <si>
-    <t>MHL</t>
-  </si>
-  <si>
-    <t>Marshall islands</t>
-  </si>
-  <si>
     <t>Belarus</t>
   </si>
   <si>
-    <t>NPL</t>
-  </si>
-  <si>
-    <t>Nepal</t>
-  </si>
-  <si>
     <t>Bermuda</t>
   </si>
   <si>
-    <t>RWA</t>
-  </si>
-  <si>
     <t>Rwanda</t>
   </si>
   <si>
     <t>Bolivia</t>
   </si>
   <si>
-    <t>SEN</t>
-  </si>
-  <si>
     <t>Senegal</t>
   </si>
   <si>
     <t>Brazil</t>
   </si>
   <si>
-    <t>SYC</t>
-  </si>
-  <si>
-    <t>Seychelles</t>
-  </si>
-  <si>
     <t>Barbados</t>
   </si>
   <si>
-    <t>SLB</t>
-  </si>
-  <si>
     <t>Solomon Islands</t>
   </si>
   <si>
     <t>Brunei Darussalam</t>
   </si>
   <si>
-    <t>TJK</t>
-  </si>
-  <si>
-    <t>Tajikistan</t>
-  </si>
-  <si>
     <t>Botswana</t>
   </si>
   <si>
-    <t>TON</t>
-  </si>
-  <si>
-    <t>Tonga</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
-    <t>VGB</t>
-  </si>
-  <si>
-    <t>British Virgin Islands</t>
-  </si>
-  <si>
     <t>Switzerland</t>
   </si>
   <si>
-    <t>NER</t>
-  </si>
-  <si>
-    <t>Niger</t>
-  </si>
-  <si>
     <t>Chile</t>
   </si>
   <si>
-    <t>TLS</t>
-  </si>
-  <si>
-    <t>Timor Leste</t>
-  </si>
-  <si>
     <t>China</t>
   </si>
   <si>
-    <t>BRN</t>
-  </si>
-  <si>
     <t>Ivory Coast</t>
   </si>
   <si>
-    <t>BEN</t>
-  </si>
-  <si>
     <t>Cameroon</t>
   </si>
   <si>
     <t>COD</t>
   </si>
   <si>
-    <t>democratic republic of the congo</t>
-  </si>
-  <si>
     <t>Congo (Democratic Republic of the)</t>
   </si>
   <si>
-    <t>GIN</t>
-  </si>
-  <si>
-    <t>Guinea</t>
-  </si>
-  <si>
-    <t>GNB</t>
-  </si>
-  <si>
-    <t>Guinea-Bissau</t>
-  </si>
-  <si>
     <t>Colombia</t>
   </si>
   <si>
-    <t>LSO</t>
-  </si>
-  <si>
-    <t>Lesotho</t>
-  </si>
-  <si>
     <t>Costa Rica</t>
   </si>
   <si>
-    <t>MLI</t>
-  </si>
-  <si>
-    <t>Mali</t>
-  </si>
-  <si>
     <t>CUW</t>
   </si>
   <si>
     <t>Curacao</t>
   </si>
   <si>
-    <t>MRT</t>
-  </si>
-  <si>
     <t>Mauritania</t>
   </si>
   <si>
     <t>Cayman Islands</t>
   </si>
   <si>
-    <t>MNG</t>
-  </si>
-  <si>
     <t>Mongolia</t>
   </si>
   <si>
@@ -460,9 +241,6 @@
   </si>
   <si>
     <t>SWZ</t>
-  </si>
-  <si>
-    <t>Eswatini</t>
   </si>
   <si>
     <t>Czech Republic</t>
@@ -4802,10 +4580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750BA387-6272-4FB3-BB91-FAD99DC88FD5}">
-  <dimension ref="A1:S185"/>
+  <dimension ref="A1:M185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4814,7 +4592,7 @@
     <col min="2" max="2" width="26.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4854,23 +4632,14 @@
       <c r="M1" s="1">
         <v>2021</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>VLOOKUP(B2,ccodes,4,FALSE)</f>
         <v>ABW</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>28</v>
@@ -4905,23 +4674,14 @@
       <c r="M2">
         <v>25</v>
       </c>
-      <c r="Q2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R2" t="s">
-        <v>7</v>
-      </c>
-      <c r="S2">
-        <v>0.34499999999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>VLOOKUP(B3,ccodes,4,FALSE)</f>
         <v>AFG</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -4956,22 +4716,13 @@
       <c r="M3">
         <v>20</v>
       </c>
-      <c r="Q3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R3" t="s">
-        <v>10</v>
-      </c>
-      <c r="S3">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>28.64</v>
@@ -5006,23 +4757,14 @@
       <c r="M4">
         <v>27.46</v>
       </c>
-      <c r="Q4" t="s">
-        <v>13</v>
-      </c>
-      <c r="R4" t="s">
-        <v>14</v>
-      </c>
-      <c r="S4">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>VLOOKUP(B5,ccodes,4,FALSE)</f>
         <v>AGO</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>35</v>
@@ -5057,41 +4799,32 @@
       <c r="M5">
         <v>25</v>
       </c>
-      <c r="Q5" t="s">
-        <v>16</v>
-      </c>
-      <c r="R5" t="s">
-        <v>17</v>
-      </c>
-      <c r="S5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>VLOOKUP(B6,ccodes,4,FALSE)</f>
         <v>AIA</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -5108,23 +4841,14 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="Q6" t="s">
-        <v>21</v>
-      </c>
-      <c r="R6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S6">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>VLOOKUP(B7,ccodes,4,FALSE)</f>
         <v>ALB</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -5159,22 +4883,13 @@
       <c r="M7">
         <v>15</v>
       </c>
-      <c r="Q7" t="s">
-        <v>24</v>
-      </c>
-      <c r="R7" t="s">
-        <v>25</v>
-      </c>
-      <c r="S7">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>29.31</v>
@@ -5209,41 +4924,32 @@
       <c r="M8">
         <v>27.19</v>
       </c>
-      <c r="Q8" t="s">
-        <v>28</v>
-      </c>
-      <c r="R8" t="s">
-        <v>29</v>
-      </c>
-      <c r="S8">
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>VLOOKUP(B9,ccodes,4,FALSE)</f>
         <v>AND</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I9">
         <v>10</v>
@@ -5260,23 +4966,14 @@
       <c r="M9">
         <v>10</v>
       </c>
-      <c r="Q9" t="s">
-        <v>31</v>
-      </c>
-      <c r="R9" t="s">
-        <v>32</v>
-      </c>
-      <c r="S9">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>VLOOKUP(B10,ccodes,4,FALSE)</f>
         <v>ARE</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>55</v>
@@ -5311,23 +5008,14 @@
       <c r="M10">
         <v>55</v>
       </c>
-      <c r="Q10" t="s">
-        <v>34</v>
-      </c>
-      <c r="R10" t="s">
-        <v>35</v>
-      </c>
-      <c r="S10">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>VLOOKUP(B11,ccodes,4,FALSE)</f>
         <v>ARG</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>35</v>
@@ -5362,23 +5050,14 @@
       <c r="M11">
         <v>25</v>
       </c>
-      <c r="Q11" t="s">
-        <v>37</v>
-      </c>
-      <c r="R11" t="s">
-        <v>38</v>
-      </c>
-      <c r="S11">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>VLOOKUP(B12,ccodes,4,FALSE)</f>
         <v>ARM</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>20</v>
@@ -5413,22 +5092,13 @@
       <c r="M12">
         <v>18</v>
       </c>
-      <c r="Q12" t="s">
-        <v>40</v>
-      </c>
-      <c r="R12" t="s">
-        <v>41</v>
-      </c>
-      <c r="S12">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="C13">
         <v>22.91</v>
@@ -5463,41 +5133,32 @@
       <c r="M13">
         <v>21.55</v>
       </c>
-      <c r="Q13" t="s">
-        <v>44</v>
-      </c>
-      <c r="R13" t="s">
-        <v>45</v>
-      </c>
-      <c r="S13">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
         <f t="shared" ref="A14:A37" si="0">VLOOKUP(B14,ccodes,4,FALSE)</f>
         <v>ATG</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H14" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I14">
         <v>25</v>
@@ -5514,23 +5175,14 @@
       <c r="M14">
         <v>25</v>
       </c>
-      <c r="Q14" t="s">
-        <v>47</v>
-      </c>
-      <c r="R14" t="s">
-        <v>48</v>
-      </c>
-      <c r="S14">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>AUS</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>30</v>
@@ -5565,23 +5217,14 @@
       <c r="M15">
         <v>30</v>
       </c>
-      <c r="Q15" t="s">
-        <v>50</v>
-      </c>
-      <c r="R15" t="s">
-        <v>51</v>
-      </c>
-      <c r="S15">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>AUT</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="C16">
         <v>25</v>
@@ -5616,41 +5259,32 @@
       <c r="M16">
         <v>25</v>
       </c>
-      <c r="Q16" t="s">
-        <v>53</v>
-      </c>
-      <c r="R16" t="s">
-        <v>54</v>
-      </c>
-      <c r="S16">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>AZE</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G17" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H17" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I17">
         <v>20</v>
@@ -5667,41 +5301,32 @@
       <c r="M17">
         <v>20</v>
       </c>
-      <c r="Q17" t="s">
-        <v>55</v>
-      </c>
-      <c r="R17" t="s">
-        <v>56</v>
-      </c>
-      <c r="S17">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>BDI</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G18" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H18" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I18">
         <v>30</v>
@@ -5718,23 +5343,14 @@
       <c r="M18">
         <v>30</v>
       </c>
-      <c r="Q18" t="s">
-        <v>58</v>
-      </c>
-      <c r="R18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S18">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>BEL</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="C19">
         <v>33.99</v>
@@ -5769,41 +5385,32 @@
       <c r="M19">
         <v>25</v>
       </c>
-      <c r="Q19" t="s">
-        <v>61</v>
-      </c>
-      <c r="R19" t="s">
-        <v>62</v>
-      </c>
-      <c r="S19">
-        <v>0.27500000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>BEN</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G20" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H20" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I20">
         <v>30</v>
@@ -5820,41 +5427,32 @@
       <c r="M20">
         <v>30</v>
       </c>
-      <c r="Q20" t="s">
-        <v>64</v>
-      </c>
-      <c r="R20" t="s">
-        <v>65</v>
-      </c>
-      <c r="S20">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>BFA</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G21" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H21" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I21">
         <v>27.5</v>
@@ -5871,23 +5469,14 @@
       <c r="M21">
         <v>28</v>
       </c>
-      <c r="Q21" t="s">
-        <v>66</v>
-      </c>
-      <c r="R21" t="s">
-        <v>67</v>
-      </c>
-      <c r="S21">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>BGD</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="C22">
         <v>27.5</v>
@@ -5922,23 +5511,14 @@
       <c r="M22">
         <v>32.5</v>
       </c>
-      <c r="Q22" t="s">
-        <v>69</v>
-      </c>
-      <c r="R22" t="s">
-        <v>70</v>
-      </c>
-      <c r="S22">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>BGR</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="C23">
         <v>10</v>
@@ -5973,23 +5553,14 @@
       <c r="M23">
         <v>10</v>
       </c>
-      <c r="Q23" t="s">
-        <v>72</v>
-      </c>
-      <c r="R23" t="s">
-        <v>73</v>
-      </c>
-      <c r="S23">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>BHR</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -6024,23 +5595,14 @@
       <c r="M24">
         <v>0</v>
       </c>
-      <c r="Q24" t="s">
-        <v>75</v>
-      </c>
-      <c r="R24" t="s">
-        <v>76</v>
-      </c>
-      <c r="S24">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>BHS</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -6075,23 +5637,14 @@
       <c r="M25">
         <v>0</v>
       </c>
-      <c r="Q25" t="s">
-        <v>78</v>
-      </c>
-      <c r="R25" t="s">
-        <v>79</v>
-      </c>
-      <c r="S25">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>BIH</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="C26">
         <v>10</v>
@@ -6126,23 +5679,14 @@
       <c r="M26">
         <v>10</v>
       </c>
-      <c r="Q26" t="s">
-        <v>81</v>
-      </c>
-      <c r="R26" t="s">
-        <v>82</v>
-      </c>
-      <c r="S26">
-        <v>0.64800000000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>BLR</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C27">
         <v>24</v>
@@ -6177,23 +5721,14 @@
       <c r="M27">
         <v>18</v>
       </c>
-      <c r="Q27" t="s">
-        <v>84</v>
-      </c>
-      <c r="R27" t="s">
-        <v>85</v>
-      </c>
-      <c r="S27">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>BMU</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -6228,23 +5763,14 @@
       <c r="M28">
         <v>0</v>
       </c>
-      <c r="Q28" t="s">
-        <v>87</v>
-      </c>
-      <c r="R28" t="s">
-        <v>88</v>
-      </c>
-      <c r="S28">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>BOL</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="C29">
         <v>25</v>
@@ -6279,23 +5805,14 @@
       <c r="M29">
         <v>25</v>
       </c>
-      <c r="Q29" t="s">
-        <v>90</v>
-      </c>
-      <c r="R29" t="s">
-        <v>91</v>
-      </c>
-      <c r="S29">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>BRA</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="C30">
         <v>34</v>
@@ -6330,23 +5847,14 @@
       <c r="M30">
         <v>34</v>
       </c>
-      <c r="Q30" t="s">
-        <v>93</v>
-      </c>
-      <c r="R30" t="s">
-        <v>94</v>
-      </c>
-      <c r="S30">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>BRB</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="C31">
         <v>25</v>
@@ -6381,41 +5889,32 @@
       <c r="M31">
         <v>5.5</v>
       </c>
-      <c r="Q31" t="s">
-        <v>96</v>
-      </c>
-      <c r="R31" t="s">
-        <v>97</v>
-      </c>
-      <c r="S31">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>BRN</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D32" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F32" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G32" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H32" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I32">
         <v>18.5</v>
@@ -6432,23 +5931,14 @@
       <c r="M32">
         <v>18.5</v>
       </c>
-      <c r="Q32" t="s">
-        <v>99</v>
-      </c>
-      <c r="R32" t="s">
-        <v>100</v>
-      </c>
-      <c r="S32">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>BWA</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="C33">
         <v>22</v>
@@ -6483,23 +5973,14 @@
       <c r="M33">
         <v>22</v>
       </c>
-      <c r="Q33" t="s">
-        <v>102</v>
-      </c>
-      <c r="R33" t="s">
-        <v>103</v>
-      </c>
-      <c r="S33">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>CAN</v>
       </c>
       <c r="B34" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="C34">
         <v>28</v>
@@ -6534,23 +6015,14 @@
       <c r="M34">
         <v>26.5</v>
       </c>
-      <c r="Q34" t="s">
-        <v>105</v>
-      </c>
-      <c r="R34" t="s">
-        <v>106</v>
-      </c>
-      <c r="S34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>CHE</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="C35">
         <v>18.309999999999999</v>
@@ -6585,23 +6057,14 @@
       <c r="M35">
         <v>14.93</v>
       </c>
-      <c r="Q35" t="s">
-        <v>108</v>
-      </c>
-      <c r="R35" t="s">
-        <v>109</v>
-      </c>
-      <c r="S35">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>CHL</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="C36">
         <v>20</v>
@@ -6636,23 +6099,14 @@
       <c r="M36">
         <v>27</v>
       </c>
-      <c r="Q36" t="s">
-        <v>111</v>
-      </c>
-      <c r="R36" t="s">
-        <v>112</v>
-      </c>
-      <c r="S36">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>CHN</v>
       </c>
       <c r="B37" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="C37">
         <v>25</v>
@@ -6687,40 +6141,31 @@
       <c r="M37">
         <v>25</v>
       </c>
-      <c r="Q37" t="s">
-        <v>114</v>
-      </c>
-      <c r="R37" t="s">
-        <v>98</v>
-      </c>
-      <c r="S37">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E38" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G38" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H38" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I38">
         <v>25</v>
@@ -6737,35 +6182,26 @@
       <c r="M38">
         <v>25</v>
       </c>
-      <c r="Q38" t="s">
-        <v>116</v>
-      </c>
-      <c r="R38" t="s">
-        <v>63</v>
-      </c>
-      <c r="S38">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
         <f>VLOOKUP(B39,ccodes,4,FALSE)</f>
         <v>CMR</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E39" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F39" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G39">
         <v>33</v>
@@ -6788,40 +6224,31 @@
       <c r="M39">
         <v>33</v>
       </c>
-      <c r="Q39" t="s">
-        <v>118</v>
-      </c>
-      <c r="R39" t="s">
-        <v>119</v>
-      </c>
-      <c r="S39">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>118</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F40" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G40" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H40" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I40">
         <v>35</v>
@@ -6838,49 +6265,40 @@
       <c r="M40">
         <v>30</v>
       </c>
-      <c r="Q40" t="s">
-        <v>121</v>
-      </c>
-      <c r="R40" t="s">
-        <v>122</v>
-      </c>
-      <c r="S40">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F41" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G41" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H41" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I41" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="J41" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="K41" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="L41">
         <v>30</v>
@@ -6888,23 +6306,14 @@
       <c r="M41">
         <v>28</v>
       </c>
-      <c r="Q41" t="s">
-        <v>123</v>
-      </c>
-      <c r="R41" t="s">
-        <v>124</v>
-      </c>
-      <c r="S41">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
         <f>VLOOKUP(B42,ccodes,4,FALSE)</f>
         <v>COL</v>
       </c>
       <c r="B42" t="s">
-        <v>125</v>
+        <v>58</v>
       </c>
       <c r="C42">
         <v>33</v>
@@ -6939,23 +6348,14 @@
       <c r="M42">
         <v>31</v>
       </c>
-      <c r="Q42" t="s">
-        <v>126</v>
-      </c>
-      <c r="R42" t="s">
-        <v>127</v>
-      </c>
-      <c r="S42">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="str">
         <f>VLOOKUP(B43,ccodes,4,FALSE)</f>
         <v>CRI</v>
       </c>
       <c r="B43" t="s">
-        <v>128</v>
+        <v>59</v>
       </c>
       <c r="C43">
         <v>30</v>
@@ -6990,22 +6390,13 @@
       <c r="M43">
         <v>30</v>
       </c>
-      <c r="Q43" t="s">
-        <v>129</v>
-      </c>
-      <c r="R43" t="s">
-        <v>130</v>
-      </c>
-      <c r="S43">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>131</v>
+        <v>60</v>
       </c>
       <c r="B44" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
       <c r="C44">
         <v>34.5</v>
@@ -7040,23 +6431,14 @@
       <c r="M44">
         <v>22</v>
       </c>
-      <c r="Q44" t="s">
-        <v>133</v>
-      </c>
-      <c r="R44" t="s">
-        <v>134</v>
-      </c>
-      <c r="S44">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
         <f t="shared" ref="A45:A58" si="1">VLOOKUP(B45,ccodes,4,FALSE)</f>
         <v>CYM</v>
       </c>
       <c r="B45" t="s">
-        <v>135</v>
+        <v>63</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -7091,23 +6473,14 @@
       <c r="M45">
         <v>0</v>
       </c>
-      <c r="Q45" t="s">
-        <v>136</v>
-      </c>
-      <c r="R45" t="s">
-        <v>137</v>
-      </c>
-      <c r="S45">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
         <f t="shared" si="1"/>
         <v>CYP</v>
       </c>
       <c r="B46" t="s">
-        <v>138</v>
+        <v>65</v>
       </c>
       <c r="C46">
         <v>10</v>
@@ -7142,23 +6515,14 @@
       <c r="M46">
         <v>12.5</v>
       </c>
-      <c r="Q46" t="s">
-        <v>139</v>
-      </c>
-      <c r="R46" t="s">
-        <v>140</v>
-      </c>
-      <c r="S46">
-        <v>0.27500000000000002</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
         <f t="shared" si="1"/>
         <v>CZE</v>
       </c>
       <c r="B47" t="s">
-        <v>141</v>
+        <v>67</v>
       </c>
       <c r="C47">
         <v>19</v>
@@ -7194,13 +6558,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
         <f t="shared" si="1"/>
         <v>DEU</v>
       </c>
       <c r="B48" t="s">
-        <v>142</v>
+        <v>68</v>
       </c>
       <c r="C48">
         <v>29.37</v>
@@ -7242,25 +6606,25 @@
         <v>DJI</v>
       </c>
       <c r="B49" t="s">
-        <v>143</v>
+        <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D49" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E49" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F49" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G49" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H49" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I49">
         <v>25</v>
@@ -7284,25 +6648,25 @@
         <v>DMA</v>
       </c>
       <c r="B50" t="s">
-        <v>144</v>
+        <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E50" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F50" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G50" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H50" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I50">
         <v>25</v>
@@ -7326,7 +6690,7 @@
         <v>DNK</v>
       </c>
       <c r="B51" t="s">
-        <v>145</v>
+        <v>71</v>
       </c>
       <c r="C51">
         <v>25</v>
@@ -7368,7 +6732,7 @@
         <v>DOM</v>
       </c>
       <c r="B52" t="s">
-        <v>146</v>
+        <v>72</v>
       </c>
       <c r="C52">
         <v>29</v>
@@ -7410,13 +6774,13 @@
         <v>DZA</v>
       </c>
       <c r="B53" t="s">
-        <v>147</v>
+        <v>73</v>
       </c>
       <c r="C53" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D53" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E53">
         <v>25</v>
@@ -7452,7 +6816,7 @@
         <v>ECU</v>
       </c>
       <c r="B54" t="s">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="C54">
         <v>24</v>
@@ -7494,7 +6858,7 @@
         <v>EGY</v>
       </c>
       <c r="B55" t="s">
-        <v>149</v>
+        <v>75</v>
       </c>
       <c r="C55">
         <v>20</v>
@@ -7536,7 +6900,7 @@
         <v>ESP</v>
       </c>
       <c r="B56" t="s">
-        <v>150</v>
+        <v>76</v>
       </c>
       <c r="C56">
         <v>30</v>
@@ -7578,7 +6942,7 @@
         <v>EST</v>
       </c>
       <c r="B57" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="C57">
         <v>21</v>
@@ -7620,25 +6984,25 @@
         <v>ETH</v>
       </c>
       <c r="B58" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="C58" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E58" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F58" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G58" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H58" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I58">
         <v>30</v>
@@ -7658,10 +7022,10 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>152</v>
+        <v>78</v>
       </c>
       <c r="B59" t="s">
-        <v>153</v>
+        <v>79</v>
       </c>
       <c r="C59">
         <v>22.58</v>
@@ -7699,10 +7063,10 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
-        <v>152</v>
+        <v>78</v>
       </c>
       <c r="B60" t="s">
-        <v>154</v>
+        <v>80</v>
       </c>
       <c r="C60">
         <v>20.83</v>
@@ -7744,7 +7108,7 @@
         <v>FIN</v>
       </c>
       <c r="B61" t="s">
-        <v>155</v>
+        <v>81</v>
       </c>
       <c r="C61">
         <v>26</v>
@@ -7786,7 +7150,7 @@
         <v>FJI</v>
       </c>
       <c r="B62" t="s">
-        <v>156</v>
+        <v>82</v>
       </c>
       <c r="C62">
         <v>28</v>
@@ -7828,7 +7192,7 @@
         <v>FRA</v>
       </c>
       <c r="B63" t="s">
-        <v>157</v>
+        <v>83</v>
       </c>
       <c r="C63">
         <v>33.33</v>
@@ -7870,25 +7234,25 @@
         <v>GAB</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="C64" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D64" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E64" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F64" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G64" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H64" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I64">
         <v>30</v>
@@ -7912,7 +7276,7 @@
         <v>GBR</v>
       </c>
       <c r="B65" t="s">
-        <v>158</v>
+        <v>84</v>
       </c>
       <c r="C65">
         <v>26</v>
@@ -7954,13 +7318,13 @@
         <v>GEO</v>
       </c>
       <c r="B66" t="s">
-        <v>159</v>
+        <v>85</v>
       </c>
       <c r="C66" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D66" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E66">
         <v>15</v>
@@ -7996,7 +7360,7 @@
         <v>GGY</v>
       </c>
       <c r="B67" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -8038,13 +7402,13 @@
         <v>GHA</v>
       </c>
       <c r="B68" t="s">
-        <v>161</v>
+        <v>87</v>
       </c>
       <c r="C68" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D68" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E68">
         <v>25</v>
@@ -8080,7 +7444,7 @@
         <v>GIB</v>
       </c>
       <c r="B69" t="s">
-        <v>162</v>
+        <v>88</v>
       </c>
       <c r="C69">
         <v>10</v>
@@ -8118,10 +7482,10 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
-        <v>163</v>
+        <v>89</v>
       </c>
       <c r="B70" t="s">
-        <v>164</v>
+        <v>90</v>
       </c>
       <c r="C70">
         <v>24.52</v>
@@ -8163,25 +7527,25 @@
         <v>GMB</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>165</v>
+        <v>91</v>
       </c>
       <c r="C71" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D71" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E71" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F71" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G71" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H71" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I71">
         <v>31</v>
@@ -8205,7 +7569,7 @@
         <v>GRC</v>
       </c>
       <c r="B72" t="s">
-        <v>166</v>
+        <v>92</v>
       </c>
       <c r="C72">
         <v>20</v>
@@ -8247,25 +7611,25 @@
         <v>GRD</v>
       </c>
       <c r="B73" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="C73" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D73" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E73" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F73" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G73" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H73" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I73">
         <v>30</v>
@@ -8289,7 +7653,7 @@
         <v>GTM</v>
       </c>
       <c r="B74" t="s">
-        <v>168</v>
+        <v>94</v>
       </c>
       <c r="C74">
         <v>31</v>
@@ -8331,7 +7695,7 @@
         <v>HKG</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>169</v>
+        <v>95</v>
       </c>
       <c r="C75">
         <v>16.5</v>
@@ -8373,7 +7737,7 @@
         <v>HND</v>
       </c>
       <c r="B76" t="s">
-        <v>170</v>
+        <v>96</v>
       </c>
       <c r="C76">
         <v>35</v>
@@ -8415,7 +7779,7 @@
         <v>HRV</v>
       </c>
       <c r="B77" t="s">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="C77">
         <v>20</v>
@@ -8457,7 +7821,7 @@
         <v>HUN</v>
       </c>
       <c r="B78" t="s">
-        <v>172</v>
+        <v>98</v>
       </c>
       <c r="C78">
         <v>19</v>
@@ -8499,7 +7863,7 @@
         <v>IDN</v>
       </c>
       <c r="B79" t="s">
-        <v>173</v>
+        <v>99</v>
       </c>
       <c r="C79">
         <v>25</v>
@@ -8541,7 +7905,7 @@
         <v>IMN</v>
       </c>
       <c r="B80" t="s">
-        <v>174</v>
+        <v>100</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -8583,7 +7947,7 @@
         <v>IND</v>
       </c>
       <c r="B81" t="s">
-        <v>175</v>
+        <v>101</v>
       </c>
       <c r="C81">
         <v>32.44</v>
@@ -8625,7 +7989,7 @@
         <v>IRL</v>
       </c>
       <c r="B82" t="s">
-        <v>176</v>
+        <v>102</v>
       </c>
       <c r="C82">
         <v>12.5</v>
@@ -8667,13 +8031,13 @@
         <v>IRQ</v>
       </c>
       <c r="B83" t="s">
-        <v>177</v>
+        <v>103</v>
       </c>
       <c r="C83" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D83" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E83">
         <v>15</v>
@@ -8709,7 +8073,7 @@
         <v>ISL</v>
       </c>
       <c r="B84" t="s">
-        <v>178</v>
+        <v>104</v>
       </c>
       <c r="C84">
         <v>20</v>
@@ -8751,7 +8115,7 @@
         <v>ISR</v>
       </c>
       <c r="B85" t="s">
-        <v>179</v>
+        <v>105</v>
       </c>
       <c r="C85">
         <v>24</v>
@@ -8793,7 +8157,7 @@
         <v>ITA</v>
       </c>
       <c r="B86" t="s">
-        <v>180</v>
+        <v>106</v>
       </c>
       <c r="C86">
         <v>31.4</v>
@@ -8835,7 +8199,7 @@
         <v>JAM</v>
       </c>
       <c r="B87" t="s">
-        <v>181</v>
+        <v>107</v>
       </c>
       <c r="C87">
         <v>33.33</v>
@@ -8877,7 +8241,7 @@
         <v>JEY</v>
       </c>
       <c r="B88" t="s">
-        <v>182</v>
+        <v>108</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -8919,7 +8283,7 @@
         <v>JOR</v>
       </c>
       <c r="B89" t="s">
-        <v>183</v>
+        <v>109</v>
       </c>
       <c r="C89">
         <v>14</v>
@@ -8961,7 +8325,7 @@
         <v>JPN</v>
       </c>
       <c r="B90" t="s">
-        <v>184</v>
+        <v>110</v>
       </c>
       <c r="C90">
         <v>40.69</v>
@@ -9003,7 +8367,7 @@
         <v>KAZ</v>
       </c>
       <c r="B91" t="s">
-        <v>185</v>
+        <v>111</v>
       </c>
       <c r="C91">
         <v>20</v>
@@ -9045,10 +8409,10 @@
         <v>KEN</v>
       </c>
       <c r="B92" t="s">
-        <v>186</v>
+        <v>112</v>
       </c>
       <c r="C92" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D92">
         <v>30</v>
@@ -9087,25 +8451,25 @@
         <v>KGZ</v>
       </c>
       <c r="B93" t="s">
-        <v>187</v>
+        <v>113</v>
       </c>
       <c r="C93" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D93" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E93" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F93" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G93" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H93" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I93">
         <v>10</v>
@@ -9129,7 +8493,7 @@
         <v>KHM</v>
       </c>
       <c r="B94" t="s">
-        <v>188</v>
+        <v>114</v>
       </c>
       <c r="C94">
         <v>20</v>
@@ -9171,25 +8535,25 @@
         <v>KNA</v>
       </c>
       <c r="B95" t="s">
-        <v>189</v>
+        <v>115</v>
       </c>
       <c r="C95" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D95" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E95" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F95" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G95" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H95" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I95">
         <v>33</v>
@@ -9209,10 +8573,10 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
-        <v>190</v>
+        <v>116</v>
       </c>
       <c r="B96" t="s">
-        <v>191</v>
+        <v>117</v>
       </c>
       <c r="C96">
         <v>22</v>
@@ -9254,7 +8618,7 @@
         <v>KWT</v>
       </c>
       <c r="B97" t="s">
-        <v>192</v>
+        <v>118</v>
       </c>
       <c r="C97">
         <v>15</v>
@@ -9292,10 +8656,10 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
-        <v>193</v>
+        <v>119</v>
       </c>
       <c r="B98" t="s">
-        <v>194</v>
+        <v>120</v>
       </c>
       <c r="C98">
         <v>28.88</v>
@@ -9337,13 +8701,13 @@
         <v>LBN</v>
       </c>
       <c r="B99" t="s">
-        <v>195</v>
+        <v>121</v>
       </c>
       <c r="C99" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D99" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E99">
         <v>15</v>
@@ -9379,7 +8743,7 @@
         <v>LBY</v>
       </c>
       <c r="B100" t="s">
-        <v>196</v>
+        <v>122</v>
       </c>
       <c r="C100">
         <v>20</v>
@@ -9421,25 +8785,25 @@
         <v>LCA</v>
       </c>
       <c r="B101" t="s">
-        <v>197</v>
+        <v>123</v>
       </c>
       <c r="C101" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D101" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E101" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F101" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G101" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H101" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I101">
         <v>30</v>
@@ -9463,7 +8827,7 @@
         <v>LIE</v>
       </c>
       <c r="B102" t="s">
-        <v>198</v>
+        <v>124</v>
       </c>
       <c r="C102">
         <v>12.5</v>
@@ -9505,7 +8869,7 @@
         <v>LKA</v>
       </c>
       <c r="B103" t="s">
-        <v>199</v>
+        <v>125</v>
       </c>
       <c r="C103">
         <v>28</v>
@@ -9547,7 +8911,7 @@
         <v>LTU</v>
       </c>
       <c r="B104" t="s">
-        <v>200</v>
+        <v>126</v>
       </c>
       <c r="C104">
         <v>15</v>
@@ -9589,7 +8953,7 @@
         <v>LUX</v>
       </c>
       <c r="B105" t="s">
-        <v>201</v>
+        <v>127</v>
       </c>
       <c r="C105">
         <v>28.8</v>
@@ -9631,7 +8995,7 @@
         <v>LVA</v>
       </c>
       <c r="B106" t="s">
-        <v>202</v>
+        <v>128</v>
       </c>
       <c r="C106">
         <v>15</v>
@@ -9673,7 +9037,7 @@
         <v>MAC</v>
       </c>
       <c r="B107" t="s">
-        <v>203</v>
+        <v>129</v>
       </c>
       <c r="C107">
         <v>12</v>
@@ -9715,13 +9079,13 @@
         <v>MAR</v>
       </c>
       <c r="B108" t="s">
-        <v>204</v>
+        <v>130</v>
       </c>
       <c r="C108" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D108" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E108">
         <v>30</v>
@@ -9757,25 +9121,25 @@
         <v>MCO</v>
       </c>
       <c r="B109" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="C109" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D109" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E109" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F109" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G109" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H109" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I109">
         <v>33.33</v>
@@ -9795,22 +9159,22 @@
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
-        <v>205</v>
+        <v>131</v>
       </c>
       <c r="B110" t="s">
-        <v>206</v>
+        <v>132</v>
       </c>
       <c r="C110" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D110" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E110" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F110" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G110">
         <v>12</v>
@@ -9840,25 +9204,25 @@
         <v>MDG</v>
       </c>
       <c r="B111" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="C111" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D111" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E111" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F111" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G111" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H111" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I111">
         <v>20</v>
@@ -9882,7 +9246,7 @@
         <v>MEX</v>
       </c>
       <c r="B112" t="s">
-        <v>207</v>
+        <v>133</v>
       </c>
       <c r="C112">
         <v>30</v>
@@ -9920,10 +9284,10 @@
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
-        <v>208</v>
+        <v>134</v>
       </c>
       <c r="B113" t="s">
-        <v>209</v>
+        <v>135</v>
       </c>
       <c r="C113">
         <v>10</v>
@@ -9965,7 +9329,7 @@
         <v>MLT</v>
       </c>
       <c r="B114" t="s">
-        <v>210</v>
+        <v>136</v>
       </c>
       <c r="C114">
         <v>35</v>
@@ -10007,25 +9371,25 @@
         <v>MMR</v>
       </c>
       <c r="B115" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C115" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D115" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E115" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F115" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G115" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H115" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I115">
         <v>25</v>
@@ -10049,7 +9413,7 @@
         <v>MNE</v>
       </c>
       <c r="B116" t="s">
-        <v>211</v>
+        <v>137</v>
       </c>
       <c r="C116">
         <v>9</v>
@@ -10091,25 +9455,25 @@
         <v>MNG</v>
       </c>
       <c r="B117" t="s">
-        <v>137</v>
+        <v>64</v>
       </c>
       <c r="C117" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D117" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E117" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F117" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G117" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H117" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I117">
         <v>25</v>
@@ -10133,7 +9497,7 @@
         <v>MOZ</v>
       </c>
       <c r="B118" t="s">
-        <v>212</v>
+        <v>138</v>
       </c>
       <c r="C118">
         <v>32</v>
@@ -10175,37 +9539,37 @@
         <v>MRT</v>
       </c>
       <c r="B119" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="C119" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D119" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E119" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F119" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G119" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H119" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I119" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="J119" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="K119" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="L119" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="M119">
         <v>25</v>
@@ -10217,7 +9581,7 @@
         <v>MUS</v>
       </c>
       <c r="B120" t="s">
-        <v>213</v>
+        <v>139</v>
       </c>
       <c r="C120">
         <v>15</v>
@@ -10259,10 +9623,10 @@
         <v>MWI</v>
       </c>
       <c r="B121" t="s">
-        <v>214</v>
+        <v>140</v>
       </c>
       <c r="C121" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D121">
         <v>30</v>
@@ -10301,7 +9665,7 @@
         <v>MYS</v>
       </c>
       <c r="B122" t="s">
-        <v>215</v>
+        <v>141</v>
       </c>
       <c r="C122">
         <v>25</v>
@@ -10343,7 +9707,7 @@
         <v>NAM</v>
       </c>
       <c r="B123" t="s">
-        <v>216</v>
+        <v>142</v>
       </c>
       <c r="C123">
         <v>34</v>
@@ -10385,7 +9749,7 @@
         <v>NGA</v>
       </c>
       <c r="B124" t="s">
-        <v>217</v>
+        <v>143</v>
       </c>
       <c r="C124">
         <v>30</v>
@@ -10427,25 +9791,25 @@
         <v>NIC</v>
       </c>
       <c r="B125" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C125" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D125" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E125" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F125" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G125" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H125" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I125">
         <v>30</v>
@@ -10469,7 +9833,7 @@
         <v>NLD</v>
       </c>
       <c r="B126" t="s">
-        <v>218</v>
+        <v>144</v>
       </c>
       <c r="C126">
         <v>25</v>
@@ -10511,7 +9875,7 @@
         <v>NOR</v>
       </c>
       <c r="B127" t="s">
-        <v>219</v>
+        <v>145</v>
       </c>
       <c r="C127">
         <v>28</v>
@@ -10549,10 +9913,10 @@
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
-        <v>220</v>
+        <v>146</v>
       </c>
       <c r="B128" t="s">
-        <v>221</v>
+        <v>147</v>
       </c>
       <c r="C128">
         <v>34</v>
@@ -10594,7 +9958,7 @@
         <v>NZL</v>
       </c>
       <c r="B129" t="s">
-        <v>222</v>
+        <v>148</v>
       </c>
       <c r="C129">
         <v>28</v>
@@ -10632,10 +9996,10 @@
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
-        <v>223</v>
+        <v>149</v>
       </c>
       <c r="B130" t="s">
-        <v>224</v>
+        <v>150</v>
       </c>
       <c r="C130">
         <v>28.6</v>
@@ -10673,10 +10037,10 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
-        <v>225</v>
+        <v>151</v>
       </c>
       <c r="B131" t="s">
-        <v>226</v>
+        <v>152</v>
       </c>
       <c r="C131">
         <v>25.42</v>
@@ -10718,7 +10082,7 @@
         <v>OMN</v>
       </c>
       <c r="B132" t="s">
-        <v>227</v>
+        <v>153</v>
       </c>
       <c r="C132">
         <v>12</v>
@@ -10760,7 +10124,7 @@
         <v>PAK</v>
       </c>
       <c r="B133" t="s">
-        <v>228</v>
+        <v>154</v>
       </c>
       <c r="C133">
         <v>35</v>
@@ -10802,7 +10166,7 @@
         <v>PAN</v>
       </c>
       <c r="B134" t="s">
-        <v>229</v>
+        <v>155</v>
       </c>
       <c r="C134">
         <v>25</v>
@@ -10844,7 +10208,7 @@
         <v>PER</v>
       </c>
       <c r="B135" t="s">
-        <v>230</v>
+        <v>156</v>
       </c>
       <c r="C135">
         <v>30</v>
@@ -10886,7 +10250,7 @@
         <v>PHL</v>
       </c>
       <c r="B136" t="s">
-        <v>231</v>
+        <v>157</v>
       </c>
       <c r="C136">
         <v>30</v>
@@ -10928,7 +10292,7 @@
         <v>PNG</v>
       </c>
       <c r="B137" t="s">
-        <v>232</v>
+        <v>158</v>
       </c>
       <c r="C137">
         <v>30</v>
@@ -10970,7 +10334,7 @@
         <v>POL</v>
       </c>
       <c r="B138" t="s">
-        <v>233</v>
+        <v>159</v>
       </c>
       <c r="C138">
         <v>19</v>
@@ -11012,7 +10376,7 @@
         <v>PRT</v>
       </c>
       <c r="B139" t="s">
-        <v>234</v>
+        <v>160</v>
       </c>
       <c r="C139">
         <v>25</v>
@@ -11054,7 +10418,7 @@
         <v>PRY</v>
       </c>
       <c r="B140" t="s">
-        <v>235</v>
+        <v>161</v>
       </c>
       <c r="C140">
         <v>10</v>
@@ -11092,28 +10456,28 @@
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="s">
-        <v>236</v>
+        <v>162</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>237</v>
+        <v>163</v>
       </c>
       <c r="C141" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D141" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E141" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F141" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G141" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H141" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I141">
         <v>15</v>
@@ -11137,7 +10501,7 @@
         <v>QAT</v>
       </c>
       <c r="B142" t="s">
-        <v>238</v>
+        <v>164</v>
       </c>
       <c r="C142">
         <v>10</v>
@@ -11176,7 +10540,7 @@
         <v>ROU</v>
       </c>
       <c r="B143" t="s">
-        <v>239</v>
+        <v>165</v>
       </c>
       <c r="C143">
         <v>16</v>
@@ -11218,7 +10582,7 @@
         <v>RUS</v>
       </c>
       <c r="B144" t="s">
-        <v>240</v>
+        <v>166</v>
       </c>
       <c r="C144">
         <v>20</v>
@@ -11260,25 +10624,25 @@
         <v>RWA</v>
       </c>
       <c r="B145" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="C145" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D145" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E145" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F145" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G145" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H145" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I145">
         <v>30</v>
@@ -11302,7 +10666,7 @@
         <v>SAU</v>
       </c>
       <c r="B146" t="s">
-        <v>241</v>
+        <v>167</v>
       </c>
       <c r="C146">
         <v>20</v>
@@ -11340,10 +10704,10 @@
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A147" s="2" t="s">
-        <v>242</v>
+        <v>168</v>
       </c>
       <c r="B147" t="s">
-        <v>243</v>
+        <v>169</v>
       </c>
       <c r="C147">
         <v>35</v>
@@ -11385,25 +10749,25 @@
         <v>SEN</v>
       </c>
       <c r="B148" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="C148" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D148" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E148" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F148" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G148" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H148" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I148">
         <v>30</v>
@@ -11427,7 +10791,7 @@
         <v>SGP</v>
       </c>
       <c r="B149" t="s">
-        <v>244</v>
+        <v>170</v>
       </c>
       <c r="C149">
         <v>17</v>
@@ -11469,25 +10833,25 @@
         <v>SLB</v>
       </c>
       <c r="B150" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="C150" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D150" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E150" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F150" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G150" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H150" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I150">
         <v>30</v>
@@ -11511,16 +10875,16 @@
         <v>SLE</v>
       </c>
       <c r="B151" t="s">
-        <v>245</v>
+        <v>171</v>
       </c>
       <c r="C151" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D151" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E151" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F151">
         <v>30</v>
@@ -11553,10 +10917,10 @@
         <v>SLV</v>
       </c>
       <c r="B152" t="s">
-        <v>246</v>
+        <v>172</v>
       </c>
       <c r="C152" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D152">
         <v>30</v>
@@ -11591,10 +10955,10 @@
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A153" s="2" t="s">
-        <v>247</v>
+        <v>173</v>
       </c>
       <c r="B153" t="s">
-        <v>248</v>
+        <v>174</v>
       </c>
       <c r="C153">
         <v>28.88</v>
@@ -11636,7 +11000,7 @@
         <v>SRB</v>
       </c>
       <c r="B154" t="s">
-        <v>249</v>
+        <v>175</v>
       </c>
       <c r="C154">
         <v>10</v>
@@ -11678,13 +11042,13 @@
         <v>SUR</v>
       </c>
       <c r="B155" t="s">
-        <v>250</v>
+        <v>176</v>
       </c>
       <c r="C155" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D155" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E155">
         <v>36</v>
@@ -11720,7 +11084,7 @@
         <v>SVK</v>
       </c>
       <c r="B156" t="s">
-        <v>251</v>
+        <v>177</v>
       </c>
       <c r="C156">
         <v>19</v>
@@ -11762,7 +11126,7 @@
         <v>SVN</v>
       </c>
       <c r="B157" t="s">
-        <v>252</v>
+        <v>178</v>
       </c>
       <c r="C157">
         <v>20</v>
@@ -11804,7 +11168,7 @@
         <v>SWE</v>
       </c>
       <c r="B158" t="s">
-        <v>253</v>
+        <v>179</v>
       </c>
       <c r="C158">
         <v>26.3</v>
@@ -11842,28 +11206,28 @@
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A159" s="2" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="B159" t="s">
-        <v>254</v>
+        <v>180</v>
       </c>
       <c r="C159" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D159" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E159" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F159" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G159" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H159" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I159">
         <v>27.5</v>
@@ -11887,7 +11251,7 @@
         <v>SXM</v>
       </c>
       <c r="B160" t="s">
-        <v>255</v>
+        <v>181</v>
       </c>
       <c r="C160">
         <v>34.5</v>
@@ -11925,22 +11289,22 @@
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A161" s="2" t="s">
-        <v>256</v>
+        <v>182</v>
       </c>
       <c r="B161" t="s">
-        <v>257</v>
+        <v>183</v>
       </c>
       <c r="C161" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D161" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E161" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F161" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G161">
         <v>24.5</v>
@@ -11966,10 +11330,10 @@
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A162" s="2" t="s">
-        <v>258</v>
+        <v>184</v>
       </c>
       <c r="B162" t="s">
-        <v>259</v>
+        <v>185</v>
       </c>
       <c r="C162">
         <v>28</v>
@@ -12007,28 +11371,28 @@
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A163" s="2" t="s">
-        <v>260</v>
+        <v>186</v>
       </c>
       <c r="B163" t="s">
-        <v>261</v>
+        <v>187</v>
       </c>
       <c r="C163" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D163" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E163" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F163" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G163" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H163" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I163">
         <v>0</v>
@@ -12052,7 +11416,7 @@
         <v>THA</v>
       </c>
       <c r="B164" t="s">
-        <v>262</v>
+        <v>188</v>
       </c>
       <c r="C164">
         <v>30</v>
@@ -12094,25 +11458,25 @@
         <v>TKM</v>
       </c>
       <c r="B165" t="s">
-        <v>263</v>
+        <v>189</v>
       </c>
       <c r="C165" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D165" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E165" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F165" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G165" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H165" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I165">
         <v>20</v>
@@ -12136,10 +11500,10 @@
         <v>TTO</v>
       </c>
       <c r="B166" t="s">
-        <v>264</v>
+        <v>190</v>
       </c>
       <c r="C166" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D166">
         <v>25</v>
@@ -12178,7 +11542,7 @@
         <v>TUN</v>
       </c>
       <c r="B167" t="s">
-        <v>265</v>
+        <v>191</v>
       </c>
       <c r="C167">
         <v>30</v>
@@ -12220,7 +11584,7 @@
         <v>TUR</v>
       </c>
       <c r="B168" t="s">
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="C168">
         <v>20</v>
@@ -12262,7 +11626,7 @@
         <v>TWN</v>
       </c>
       <c r="B169" t="s">
-        <v>267</v>
+        <v>193</v>
       </c>
       <c r="C169">
         <v>17</v>
@@ -12304,7 +11668,7 @@
         <v>TZA</v>
       </c>
       <c r="B170" t="s">
-        <v>268</v>
+        <v>194</v>
       </c>
       <c r="C170">
         <v>30</v>
@@ -12346,7 +11710,7 @@
         <v>UGA</v>
       </c>
       <c r="B171" t="s">
-        <v>269</v>
+        <v>195</v>
       </c>
       <c r="C171">
         <v>30</v>
@@ -12388,7 +11752,7 @@
         <v>UKR</v>
       </c>
       <c r="B172" t="s">
-        <v>270</v>
+        <v>196</v>
       </c>
       <c r="C172">
         <v>25</v>
@@ -12430,7 +11794,7 @@
         <v>URY</v>
       </c>
       <c r="B173" t="s">
-        <v>271</v>
+        <v>197</v>
       </c>
       <c r="C173">
         <v>25</v>
@@ -12472,7 +11836,7 @@
         <v>USA</v>
       </c>
       <c r="B174" t="s">
-        <v>272</v>
+        <v>198</v>
       </c>
       <c r="C174">
         <v>40</v>
@@ -12514,22 +11878,22 @@
         <v>UZB</v>
       </c>
       <c r="B175" t="s">
-        <v>273</v>
+        <v>199</v>
       </c>
       <c r="C175" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D175" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E175" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F175" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G175" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H175">
         <v>7.5</v>
@@ -12556,25 +11920,25 @@
         <v>VCT</v>
       </c>
       <c r="B176" t="s">
-        <v>274</v>
+        <v>200</v>
       </c>
       <c r="C176" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D176" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E176" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F176" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G176" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H176" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I176">
         <v>32.5</v>
@@ -12598,7 +11962,7 @@
         <v>VEN</v>
       </c>
       <c r="B177" t="s">
-        <v>275</v>
+        <v>201</v>
       </c>
       <c r="C177">
         <v>34</v>
@@ -12640,7 +12004,7 @@
         <v>VNM</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>276</v>
+        <v>202</v>
       </c>
       <c r="C178">
         <v>25</v>
@@ -12682,7 +12046,7 @@
         <v>VUT</v>
       </c>
       <c r="B179" t="s">
-        <v>277</v>
+        <v>203</v>
       </c>
       <c r="C179">
         <v>0</v>
@@ -12724,7 +12088,7 @@
         <v>WSM</v>
       </c>
       <c r="B180" t="s">
-        <v>278</v>
+        <v>204</v>
       </c>
       <c r="C180">
         <v>27</v>
@@ -12766,7 +12130,7 @@
         <v>YEM</v>
       </c>
       <c r="B181" t="s">
-        <v>279</v>
+        <v>205</v>
       </c>
       <c r="C181">
         <v>20</v>
@@ -12808,7 +12172,7 @@
         <v>ZAF</v>
       </c>
       <c r="B182" t="s">
-        <v>280</v>
+        <v>206</v>
       </c>
       <c r="C182">
         <v>34.549999999999997</v>
@@ -12850,7 +12214,7 @@
         <v>ZMB</v>
       </c>
       <c r="B183" t="s">
-        <v>281</v>
+        <v>207</v>
       </c>
       <c r="C183">
         <v>35</v>
@@ -12892,7 +12256,7 @@
         <v>ZWE</v>
       </c>
       <c r="B184" t="s">
-        <v>282</v>
+        <v>208</v>
       </c>
       <c r="C184">
         <v>25.75</v>
@@ -12934,10 +12298,10 @@
         <v>#N/A</v>
       </c>
       <c r="B185" t="s">
-        <v>283</v>
+        <v>209</v>
       </c>
       <c r="C185" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D185">
         <v>0</v>

</xml_diff>